<commit_message>
commit for temporary work after factest worked
</commit_message>
<xml_diff>
--- a/docs/Auto_SEE_ACC.xlsx
+++ b/docs/Auto_SEE_ACC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProjects\Cartel\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProjects\Vendetta\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2457,12 +2457,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2553,7 +2552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
@@ -2578,7 +2577,7 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -2603,7 +2602,7 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -2628,7 +2627,7 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>29</v>
       </c>
@@ -2653,7 +2652,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
@@ -2678,7 +2677,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>39</v>
       </c>
@@ -2703,7 +2702,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>43</v>
       </c>
@@ -2728,7 +2727,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>47</v>
       </c>
@@ -2753,7 +2752,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>51</v>
       </c>
@@ -2778,7 +2777,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>55</v>
       </c>
@@ -2853,7 +2852,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>68</v>
       </c>
@@ -2878,7 +2877,7 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>73</v>
       </c>
@@ -2903,7 +2902,7 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>77</v>
       </c>
@@ -2928,7 +2927,7 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>81</v>
       </c>
@@ -2953,7 +2952,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" ht="216" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>85</v>
       </c>
@@ -2978,7 +2977,7 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>88</v>
       </c>
@@ -3003,7 +3002,7 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" ht="216" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>91</v>
       </c>
@@ -3028,7 +3027,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>94</v>
       </c>
@@ -3053,7 +3052,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" ht="216" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>97</v>
       </c>
@@ -3078,7 +3077,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>100</v>
       </c>
@@ -3103,7 +3102,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="1:9" ht="216" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>103</v>
       </c>
@@ -3128,7 +3127,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="1:9" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>106</v>
       </c>
@@ -3660,13 +3659,7 @@
       <c r="I73" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H27">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Internal Concurrency"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:H27"/>
   <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.33</formula>

</xml_diff>